<commit_message>
Add Ca_conc forcing from 600 to 2800 Ma Data from Hardie-2003 Geology
</commit_message>
<xml_diff>
--- a/src/Forcings/Horita_Ca.xlsx
+++ b/src/Forcings/Horita_Ca.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liziheng/Documents/Julia/PALEOcopse.jl/src/Forcings/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A09A042-B935-C347-B85E-54105EF40D2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="500" yWindow="2220" windowWidth="17080" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,13 +33,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -57,14 +70,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -72,12 +88,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -119,7 +138,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -152,9 +171,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -187,6 +223,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -362,16 +415,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -379,343 +432,706 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:2">
+      <c r="A2" s="2">
+        <v>2800</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.1609687542281524</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2">
+        <v>2650</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.5581422754114675</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2">
+        <v>2600</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2.1298975641478881</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2">
+        <v>2550</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2.2128239037356137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2">
+        <v>2500</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2.0818875780707842</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2">
+        <v>2450</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.9116703547065061</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2">
+        <v>2400</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.7196304103980902</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2">
+        <v>2375</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.6454331591880205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2">
+        <v>2350</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.309363256648292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2">
+        <v>2300</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1.1085942239622204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2">
+        <v>2250</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.1609687542281524</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="2">
+        <v>2200</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.1871560193611179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="2">
+        <v>2150</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.309363256648292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="2">
+        <v>2100</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.902941266328851</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="2">
+        <v>2050</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1.929128531461817</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1.501403200956708</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2">
+        <v>1950</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1.4075655008969139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2">
+        <v>1900</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.501403200956708</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="2">
+        <v>1850</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1.9465867082171275</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2">
+        <v>1800</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2.1997302711691304</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="2">
+        <v>1750</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2.2608338898127172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="2">
+        <v>1700</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2.2608338898127172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="2">
+        <v>1650</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1.3420973380644994</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2">
+        <v>1600</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1.4577577590684316</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="2">
+        <v>1550</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1.2220723728717391</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1.1609687542281524</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="2">
+        <v>1450</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1.4075655008969139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="2">
+        <v>1400</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1.854931280251747</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="2">
+        <v>1350</v>
+      </c>
+      <c r="B30" s="2">
+        <v>2.0076903268607142</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="2">
+        <v>1300</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1.5581422754114675</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="2">
+        <v>1250</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1.1609687542281524</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="2">
+        <v>1200</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1.1609687542281524</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="2">
+        <v>1150</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1.309363256648292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="2">
+        <v>1130</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1.3791959636695343</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="2">
+        <v>1110</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1.5843295405444331</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="2">
+        <v>1100</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1.7632758522863665</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="2">
+        <v>1085</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1.929128531461817</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="2">
+        <v>1045</v>
+      </c>
+      <c r="B39" s="2">
+        <v>2.1604493734696817</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="2">
+        <v>1010</v>
+      </c>
+      <c r="B40" s="2">
+        <v>2.3961347596663742</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="2">
+        <v>985</v>
+      </c>
+      <c r="B41" s="2">
+        <v>2.4048638480440299</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="2">
+        <v>965</v>
+      </c>
+      <c r="B42" s="2">
+        <v>2.3961347596663742</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="2">
+        <v>950</v>
+      </c>
+      <c r="B43" s="2">
+        <v>2.1604493734696817</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="2">
+        <v>900</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1.492674112579053</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="2">
+        <v>850</v>
+      </c>
+      <c r="B45" s="2">
+        <v>1.1609687542281524</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="2">
+        <v>750</v>
+      </c>
+      <c r="B46" s="2">
+        <v>1.0300324285633231</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47">
         <v>600</v>
       </c>
-      <c r="B2">
+      <c r="B47">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="48" spans="1:2">
+      <c r="A48" s="1">
         <v>546.88524590163934</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B48" s="1">
         <v>0.95337864854058263</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="49" spans="1:2">
+      <c r="A49" s="1">
         <v>540.98360655737702</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B49" s="1">
         <v>1.2463014794082354</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="50" spans="1:2">
+      <c r="A50" s="1">
         <v>529.18032786885249</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B50" s="1">
         <v>1.7101959216313458</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="51" spans="1:2">
+      <c r="A51" s="1">
         <v>519.34426229508199</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B51" s="1">
         <v>2.052059176329466</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="52" spans="1:2">
+      <c r="A52" s="1">
         <v>507.5409836065574</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B52" s="1">
         <v>2.3208316673330645</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="53" spans="1:2">
+      <c r="A53" s="1">
         <v>491.80327868852459</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B53" s="1">
         <v>2.4922031187524962</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="54" spans="1:2">
+      <c r="A54" s="1">
         <v>468.19672131147536</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B54" s="1">
         <v>2.5907237105157908</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="55" spans="1:2">
+      <c r="A55" s="1">
         <v>430.81967213114751</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B55" s="1">
         <v>2.6842431027588987</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="56" spans="1:2">
+      <c r="A56" s="1">
         <v>397.37704918032784</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B56" s="1">
         <v>2.7155537784886015</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="57" spans="1:2">
+      <c r="A57" s="1">
         <v>385.57377049180326</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B57" s="1">
         <v>2.7160335865653709</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="58" spans="1:2">
+      <c r="A58" s="1">
         <v>369.8360655737705</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B58" s="1">
         <v>2.6678928428628517</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="59" spans="1:2">
+      <c r="A59" s="1">
         <v>361.96721311475414</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B59" s="1">
         <v>2.5950419832067149</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    <row r="60" spans="1:2">
+      <c r="A60" s="1">
         <v>352.13114754098365</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B60" s="1">
         <v>2.4978808476609329</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+    <row r="61" spans="1:2">
+      <c r="A61" s="1">
         <v>340.32786885245906</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B61" s="1">
         <v>2.2788484606157513</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+    <row r="62" spans="1:2">
+      <c r="A62" s="1">
         <v>334.42622950819668</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B62" s="1">
         <v>2.1815273890443798</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+    <row r="63" spans="1:2">
+      <c r="A63" s="1">
         <v>320.65573770491807</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B63" s="1">
         <v>1.8162335065973592</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+    <row r="64" spans="1:2">
+      <c r="A64" s="1">
         <v>316.72131147540983</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B64" s="1">
         <v>1.6944422231107537</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+    <row r="65" spans="1:2">
+      <c r="A65" s="1">
         <v>297.04918032786884</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B65" s="1">
         <v>1.4025589764094348</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+    <row r="66" spans="1:2">
+      <c r="A66" s="1">
         <v>289.18032786885249</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B66" s="1">
         <v>1.2809276289484193</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+    <row r="67" spans="1:2">
+      <c r="A67" s="1">
         <v>277.3770491803279</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B67" s="1">
         <v>1.1594562175129937</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+    <row r="68" spans="1:2">
+      <c r="A68" s="1">
         <v>261.63934426229508</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B68" s="1">
         <v>1.0625349860055966</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+    <row r="69" spans="1:2">
+      <c r="A69" s="1">
         <v>253.7704918032787</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B69" s="1">
         <v>1.0384646141543372</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+    <row r="70" spans="1:2">
+      <c r="A70" s="1">
         <v>240</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B70" s="1">
         <v>1.1121951219512183</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+    <row r="71" spans="1:2">
+      <c r="A71" s="1">
         <v>228.19672131147541</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B71" s="1">
         <v>1.2590163934426215</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+    <row r="72" spans="1:2">
+      <c r="A72" s="1">
         <v>222.29508196721312</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B72" s="1">
         <v>1.3568172730907622</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+    <row r="73" spans="1:2">
+      <c r="A73" s="1">
         <v>206.55737704918033</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B73" s="1">
         <v>1.6989204318272675</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+    <row r="74" spans="1:2">
+      <c r="A74" s="1">
         <v>196.72131147540983</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B74" s="1">
         <v>1.8456617353058757</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+    <row r="75" spans="1:2">
+      <c r="A75" s="1">
         <v>171.14754098360658</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B75" s="1">
         <v>2.0906037584965991</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+    <row r="76" spans="1:2">
+      <c r="A76" s="1">
         <v>163.27868852459017</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B76" s="1">
         <v>2.1397041183526566</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+    <row r="77" spans="1:2">
+      <c r="A77" s="1">
         <v>139.67213114754097</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B77" s="1">
         <v>2.165053978408634</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+    <row r="78" spans="1:2">
+      <c r="A78" s="1">
         <v>125.90163934426229</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B78" s="1">
         <v>2.1168332666933205</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+    <row r="79" spans="1:2">
+      <c r="A79" s="1">
         <v>100.32786885245902</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B79" s="1">
         <v>2.0203118752498983</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+    <row r="80" spans="1:2">
+      <c r="A80" s="1">
         <v>90.491803278688536</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B80" s="1">
         <v>1.9719312275089944</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+    <row r="81" spans="1:2">
+      <c r="A81" s="1">
         <v>62.950819672131146</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B81" s="1">
         <v>1.8023190723710496</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+    <row r="82" spans="1:2">
+      <c r="A82" s="1">
         <v>55.081967213114751</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B82" s="1">
         <v>1.7294682127149124</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+    <row r="83" spans="1:2">
+      <c r="A83" s="1">
         <v>27.540983606557376</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B83" s="1">
         <v>1.4379048380647728</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+    <row r="84" spans="1:2">
+      <c r="A84" s="1">
         <v>19.672131147540984</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B84" s="1">
         <v>1.340663734506196</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+    <row r="85" spans="1:2">
+      <c r="A85" s="1">
         <v>0</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B85" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>